<commit_message>
Gantt Chart Update, User Manual, Ui Function Implementation
</commit_message>
<xml_diff>
--- a/Documentation/Gantt chart.xlsx
+++ b/Documentation/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\2808ICT\2808ICT Assignment Version 2\ST_Assignment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\2808ICT\2808ICT Assignment Version 2\ST_Assignment1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EE1AD5-9871-4D0E-8A59-FFEF8EB8FDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F34D9C-57D7-4048-B8AA-44FB6B6A5BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6045" yWindow="3585" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -691,6 +691,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -749,7 +758,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -832,6 +841,27 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -853,33 +883,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1395,8 +1408,8 @@
   </sheetPr>
   <dimension ref="B1:BP41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1431,13 +1444,13 @@
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
       <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1445,37 +1458,37 @@
         <v>1</v>
       </c>
       <c r="K2" s="24"/>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="34"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="32" t="s">
+      <c r="R2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="41"/>
       <c r="V2" s="26"/>
-      <c r="W2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="37"/>
+      <c r="W2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="44"/>
       <c r="AA2" s="27"/>
-      <c r="AB2" s="35" t="s">
+      <c r="AB2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="37"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
+      <c r="AF2" s="43"/>
+      <c r="AG2" s="43"/>
+      <c r="AH2" s="44"/>
       <c r="AI2" s="31"/>
       <c r="AJ2" s="12" t="s">
         <v>3</v>
@@ -1498,61 +1511,63 @@
       <c r="I3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="45" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="36"/>
+      <c r="AG3" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="AH3" s="46"/>
-      <c r="AI3" s="46"/>
-      <c r="AJ3" s="46"/>
-      <c r="AK3" s="46"/>
-      <c r="AL3" s="46"/>
-      <c r="AM3" s="46"/>
-      <c r="AN3" s="46"/>
-      <c r="AO3" s="46"/>
-      <c r="AP3" s="46"/>
-      <c r="AQ3" s="46"/>
-      <c r="AR3" s="46"/>
-      <c r="AS3" s="46"/>
-      <c r="AT3" s="46"/>
-      <c r="AU3" s="46"/>
-      <c r="AV3" s="46"/>
-      <c r="AW3" s="46"/>
-      <c r="AX3" s="46"/>
-      <c r="AY3" s="46"/>
-      <c r="AZ3" s="46"/>
-      <c r="BA3" s="47"/>
-      <c r="BB3" s="45" t="s">
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="35"/>
+      <c r="AK3" s="35"/>
+      <c r="AL3" s="35"/>
+      <c r="AM3" s="35"/>
+      <c r="AN3" s="35"/>
+      <c r="AO3" s="35"/>
+      <c r="AP3" s="35"/>
+      <c r="AQ3" s="35"/>
+      <c r="AR3" s="35"/>
+      <c r="AS3" s="35"/>
+      <c r="AT3" s="35"/>
+      <c r="AU3" s="35"/>
+      <c r="AV3" s="35"/>
+      <c r="AW3" s="35"/>
+      <c r="AX3" s="35"/>
+      <c r="AY3" s="35"/>
+      <c r="AZ3" s="35"/>
+      <c r="BA3" s="35"/>
+      <c r="BB3" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="BC3" s="46"/>
-      <c r="BD3" s="46"/>
-      <c r="BE3" s="46"/>
-      <c r="BF3" s="47"/>
+      <c r="BC3" s="35"/>
+      <c r="BD3" s="35"/>
+      <c r="BE3" s="35"/>
+      <c r="BF3" s="35"/>
+      <c r="BG3" s="35"/>
+      <c r="BH3" s="36"/>
     </row>
     <row r="4" spans="2:68" ht="17.25" x14ac:dyDescent="0.25">
       <c r="C4" s="11"/>
@@ -1693,126 +1708,134 @@
       <c r="AZ4" s="29">
         <v>28</v>
       </c>
-      <c r="BA4" s="30">
+      <c r="BA4" s="29">
         <v>29</v>
       </c>
-      <c r="BB4" s="28">
+      <c r="BB4" s="50">
         <v>2</v>
       </c>
-      <c r="BC4" s="29">
+      <c r="BC4" s="49">
         <v>3</v>
       </c>
-      <c r="BD4" s="29">
+      <c r="BD4" s="49">
         <v>4</v>
       </c>
-      <c r="BE4" s="29">
+      <c r="BE4" s="49">
         <v>5</v>
       </c>
-      <c r="BF4" s="30">
+      <c r="BF4" s="49">
         <v>6</v>
       </c>
+      <c r="BG4" s="48">
+        <v>7</v>
+      </c>
+      <c r="BH4" s="51">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="2:68" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="45" t="s">
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="45" t="s">
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="47"/>
-      <c r="X5" s="45" t="s">
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="36"/>
+      <c r="X5" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="Y5" s="46"/>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="45" t="s">
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="36"/>
+      <c r="AC5" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="46"/>
-      <c r="AG5" s="47"/>
-      <c r="AH5" s="45" t="s">
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="36"/>
+      <c r="AH5" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="AI5" s="46"/>
-      <c r="AJ5" s="46"/>
-      <c r="AK5" s="46"/>
-      <c r="AL5" s="47"/>
-      <c r="AM5" s="45" t="s">
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="36"/>
+      <c r="AM5" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="AN5" s="46"/>
-      <c r="AO5" s="46"/>
-      <c r="AP5" s="46"/>
-      <c r="AQ5" s="47"/>
-      <c r="AR5" s="45" t="s">
+      <c r="AN5" s="35"/>
+      <c r="AO5" s="35"/>
+      <c r="AP5" s="35"/>
+      <c r="AQ5" s="36"/>
+      <c r="AR5" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="AS5" s="46"/>
-      <c r="AT5" s="46"/>
-      <c r="AU5" s="46"/>
-      <c r="AV5" s="47"/>
-      <c r="AW5" s="45" t="s">
+      <c r="AS5" s="35"/>
+      <c r="AT5" s="35"/>
+      <c r="AU5" s="35"/>
+      <c r="AV5" s="36"/>
+      <c r="AW5" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="46"/>
-      <c r="AZ5" s="46"/>
-      <c r="BA5" s="47"/>
-      <c r="BB5" s="45" t="s">
+      <c r="AX5" s="35"/>
+      <c r="AY5" s="35"/>
+      <c r="AZ5" s="35"/>
+      <c r="BA5" s="35"/>
+      <c r="BB5" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="BC5" s="46"/>
-      <c r="BD5" s="46"/>
-      <c r="BE5" s="46"/>
-      <c r="BF5" s="47"/>
+      <c r="BC5" s="35"/>
+      <c r="BD5" s="35"/>
+      <c r="BE5" s="35"/>
+      <c r="BF5" s="35"/>
+      <c r="BG5" s="35"/>
+      <c r="BH5" s="36"/>
     </row>
     <row r="6" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="44"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="18">
         <v>1</v>
       </c>
@@ -1945,7 +1968,7 @@
       <c r="AZ6" s="19">
         <v>44</v>
       </c>
-      <c r="BA6" s="20">
+      <c r="BA6" s="19">
         <v>45</v>
       </c>
       <c r="BB6" s="18">
@@ -1960,13 +1983,13 @@
       <c r="BE6" s="19">
         <v>49</v>
       </c>
-      <c r="BF6" s="20">
+      <c r="BF6" s="19">
         <v>50</v>
       </c>
-      <c r="BG6" s="3">
+      <c r="BG6" s="19">
         <v>51</v>
       </c>
-      <c r="BH6" s="3">
+      <c r="BH6" s="20">
         <v>52</v>
       </c>
       <c r="BI6" s="3">
@@ -2007,9 +2030,11 @@
       <c r="F7" s="6">
         <v>9</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6">
+        <v>44</v>
+      </c>
       <c r="H7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2278,10 +2303,14 @@
       <c r="E19" s="17">
         <v>10</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="F19" s="6">
+        <v>31</v>
+      </c>
+      <c r="G19" s="6">
+        <v>22</v>
+      </c>
       <c r="H19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2297,10 +2326,14 @@
       <c r="E20" s="17">
         <v>10</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="F20" s="6">
+        <v>31</v>
+      </c>
+      <c r="G20" s="6">
+        <v>22</v>
+      </c>
       <c r="H20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2316,10 +2349,14 @@
       <c r="E21" s="17">
         <v>5</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="6">
+        <v>31</v>
+      </c>
+      <c r="G21" s="6">
+        <v>22</v>
+      </c>
       <c r="H21" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2335,10 +2372,14 @@
       <c r="E22" s="17">
         <v>3</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="F22" s="6">
+        <v>31</v>
+      </c>
+      <c r="G22" s="6">
+        <v>22</v>
+      </c>
       <c r="H22" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2354,10 +2395,14 @@
       <c r="E23" s="17">
         <v>1</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="F23" s="6">
+        <v>52</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
       <c r="H23" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2373,10 +2418,14 @@
       <c r="E24" s="17">
         <v>1</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="F24" s="6">
+        <v>52</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
       <c r="H24" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2392,10 +2441,14 @@
       <c r="E25" s="17">
         <v>10</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="F25" s="6">
+        <v>41</v>
+      </c>
+      <c r="G25" s="6">
+        <v>12</v>
+      </c>
       <c r="H25" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2411,10 +2464,14 @@
       <c r="E26" s="17">
         <v>4</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="F26" s="6">
+        <v>41</v>
+      </c>
+      <c r="G26" s="6">
+        <v>12</v>
+      </c>
       <c r="H26" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2430,10 +2487,14 @@
       <c r="E27" s="17">
         <v>4</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+      <c r="F27" s="6">
+        <v>41</v>
+      </c>
+      <c r="G27" s="6">
+        <v>12</v>
+      </c>
       <c r="H27" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2449,10 +2510,14 @@
       <c r="E28" s="17">
         <v>1</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+      <c r="F28" s="6">
+        <v>52</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
       <c r="H28" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2468,10 +2533,14 @@
       <c r="E29" s="17">
         <v>1</v>
       </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="F29" s="6">
+        <v>52</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
       <c r="H29" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2487,10 +2556,14 @@
       <c r="E30" s="17">
         <v>1</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="F30" s="6">
+        <v>52</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
       <c r="H30" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2562,10 +2635,20 @@
     <row r="41" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="BB3:BH3"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="L2:P2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="J3:AF3"/>
     <mergeCell ref="AG3:BA3"/>
-    <mergeCell ref="BB3:BF3"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="N5:R5"/>
     <mergeCell ref="S5:W5"/>
@@ -2575,18 +2658,8 @@
     <mergeCell ref="AM5:AQ5"/>
     <mergeCell ref="AR5:AV5"/>
     <mergeCell ref="AW5:BA5"/>
-    <mergeCell ref="BB5:BF5"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="F5:F6"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="L2:P2"/>
   </mergeCells>
   <conditionalFormatting sqref="A31:A41">
     <cfRule type="expression" dxfId="16" priority="21">

</xml_diff>